<commit_message>
arreglos en los modelos
</commit_message>
<xml_diff>
--- a/salidas/variables_importances.xlsx
+++ b/salidas/variables_importances.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.1331788926662452</v>
+        <v>0.1239759412439982</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.02834630514734566</v>
+        <v>0.02449280966617213</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.09263329241656489</v>
+        <v>0.09640633152972077</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.06279447429805823</v>
+        <v>0.0509324021375486</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.05262773572640934</v>
+        <v>0.05642321045469301</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.03163597190638677</v>
+        <v>0.03459464430895638</v>
       </c>
     </row>
     <row r="8">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.1506221329266786</v>
+        <v>0.1643618244236488</v>
       </c>
     </row>
     <row r="9">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.06745114382928027</v>
+        <v>0.06470733700590128</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.09346993769728408</v>
+        <v>0.09134663100090497</v>
       </c>
     </row>
     <row r="11">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.0888596538614522</v>
+        <v>0.09805506186326893</v>
       </c>
     </row>
     <row r="12">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.08441507892815733</v>
+        <v>0.07945235310024075</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.05870846728521958</v>
+        <v>0.05254426393812136</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.05525691331091791</v>
+        <v>0.0627071893268247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se le agrego la el desicion tree
</commit_message>
<xml_diff>
--- a/salidas/variables_importances.xlsx
+++ b/salidas/variables_importances.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.1239759412439982</v>
+        <v>0.1247905694626398</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.02449280966617213</v>
+        <v>0.02661499342593231</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.09640633152972077</v>
+        <v>0.0933881345806391</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0509324021375486</v>
+        <v>0.06643477924217901</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.05642321045469301</v>
+        <v>0.05695587007455943</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.03459464430895638</v>
+        <v>0.0339732674219591</v>
       </c>
     </row>
     <row r="8">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.1643618244236488</v>
+        <v>0.1592739769840469</v>
       </c>
     </row>
     <row r="9">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.06470733700590128</v>
+        <v>0.07245769372894408</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.09134663100090497</v>
+        <v>0.07920502053931509</v>
       </c>
     </row>
     <row r="11">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.09805506186326893</v>
+        <v>0.09925769745512135</v>
       </c>
     </row>
     <row r="12">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.07945235310024075</v>
+        <v>0.08328591025254585</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.05254426393812136</v>
+        <v>0.05339220446728885</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.0627071893268247</v>
+        <v>0.05096988236482914</v>
       </c>
     </row>
   </sheetData>

</xml_diff>